<commit_message>
Frontrnd updated and sample excel for importing users, updated
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33013252-E28A-4038-87A0-C18322376DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>userId*</t>
   </si>
@@ -107,6 +107,18 @@
   </si>
   <si>
     <t>09123456789</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>#Parrsoo2020#</t>
+  </si>
+  <si>
+    <t>1400/10/20 13:13:13.259</t>
+  </si>
+  <si>
+    <t>alit</t>
   </si>
 </sst>
 </file>
@@ -122,16 +134,19 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -430,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -442,10 +457,12 @@
     <col min="6" max="6" width="18.6796875" customWidth="1"/>
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="42.453125" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" customWidth="1"/>
+    <col min="12" max="12" width="21.54296875" customWidth="1"/>
+    <col min="13" max="13" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,13 +496,16 @@
       <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -514,71 +534,76 @@
       <c r="J2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="L6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="L7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B8" s="7"/>
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="L8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L10" s="10" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M10" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L11" s="10" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L12" s="10" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M12" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L13" s="11"/>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="M13" s="11"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Importing users, if groups not exist, won't be create and prompt user and some minor fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1280A350-7C4A-47E3-98EB-E1BECD7E1172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>1234568sda</t>
   </si>
   <si>
-    <t>1598656906150, 1598656906151</t>
-  </si>
-  <si>
     <t>09123456789</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>alit</t>
+  </si>
+  <si>
+    <t>Staff, Managers</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -497,7 +497,7 @@
         <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>9</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -517,13 +517,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
@@ -535,10 +535,10 @@
         <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
End Time Problem Fixed. new frontend added
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1280A350-7C4A-47E3-98EB-E1BECD7E1172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -103,6 +103,9 @@
     <t>1234568sda</t>
   </si>
   <si>
+    <t>1598656906150, 1598656906151</t>
+  </si>
+  <si>
     <t>09123456789</t>
   </si>
   <si>
@@ -116,9 +119,6 @@
   </si>
   <si>
     <t>alit</t>
-  </si>
-  <si>
-    <t>Staff, Managers</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -497,7 +497,7 @@
         <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>9</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -517,13 +517,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
@@ -535,10 +535,10 @@
         <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
New xlsx file for users added. refresh users and sync users problem, fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82179E1-20F9-4C20-8494-8704936D18C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>1234568sda</t>
   </si>
   <si>
-    <t>1598656906150, 1598656906151</t>
-  </si>
-  <si>
     <t>09123456789</t>
   </si>
   <si>
@@ -115,10 +112,13 @@
     <t>#Parrsoo2020#</t>
   </si>
   <si>
-    <t>1400/10/20 13:13:13.259</t>
-  </si>
-  <si>
-    <t>alit</t>
+    <t>Staff, Students</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>1400-10-20 13:13:13.259</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -497,7 +497,7 @@
         <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>9</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -517,28 +517,28 @@
         <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Some minor changes in user update
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maziyar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF4723-D175-41DC-A7E3-8196C68684B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4949572-485C-4E44-AD45-16B10E49BAA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13710" yWindow="1770" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>userId*</t>
   </si>
@@ -67,9 +67,6 @@
     <t>توضیحات</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>مثال: (این سطر پاک شود)</t>
   </si>
   <si>
@@ -88,12 +85,6 @@
     <t>مقادیر status در صورتی که مقادیر زیر وارد شود معتبر است:</t>
   </si>
   <si>
-    <t>disabled</t>
-  </si>
-  <si>
-    <t>locked</t>
-  </si>
-  <si>
     <t>employeeNumber</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>1234568sda</t>
   </si>
   <si>
-    <t>1598656906150, 1598656906151</t>
-  </si>
-  <si>
     <t>09123456789</t>
   </si>
   <si>
@@ -115,10 +103,16 @@
     <t>#Parrsoo2020#</t>
   </si>
   <si>
-    <t>1400/10/20 13:13:13.259</t>
-  </si>
-  <si>
-    <t>alit</t>
+    <t>disable</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>Manager, Staff</t>
+  </si>
+  <si>
+    <t>1400-10-20 13:13:13.259</t>
   </si>
 </sst>
 </file>
@@ -447,14 +441,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="5" max="5" width="11.2265625" style="14"/>
     <col min="6" max="6" width="18.6796875" customWidth="1"/>
+    <col min="7" max="7" width="15.40625" customWidth="1"/>
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="12.36328125" customWidth="1"/>
@@ -491,13 +486,13 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>9</v>
@@ -505,7 +500,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -517,31 +512,31 @@
         <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
@@ -555,21 +550,21 @@
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
       <c r="M5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
       <c r="M6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
       <c r="M7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.5">
@@ -577,30 +572,28 @@
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
       <c r="M8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
       <c r="M9" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="M10" s="10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="M11" s="10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M12" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="M13" s="11"/>

</xml_diff>

<commit_message>
Minor fixes in create and update users
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4949572-485C-4E44-AD45-16B10E49BAA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FDB0A-C179-4492-B476-D3B52344C18F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,10 +109,10 @@
     <t>enable</t>
   </si>
   <si>
-    <t>Manager, Staff</t>
-  </si>
-  <si>
     <t>1400-10-20 13:13:13.259</t>
+  </si>
+  <si>
+    <t>Managers, Staff</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -518,7 +518,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
@@ -533,7 +533,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Minor fix for showing 302 error password(repetitive). EndTime removed from users.xlsx file.
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da1933711cb19495/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FDB0A-C179-4492-B476-D3B52344C18F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C2067E39-2B06-4FD4-A39F-3B3C2D2880FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A20464F-D34E-4517-ADCE-4C3E5165109D}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>userId*</t>
   </si>
@@ -52,67 +52,61 @@
     <t>این سطر را پاک نکنید(Don't remove)</t>
   </si>
   <si>
+    <t>amiri</t>
+  </si>
+  <si>
+    <t>علی امیری</t>
+  </si>
+  <si>
+    <t>ali.amiri@yahoo.com</t>
+  </si>
+  <si>
+    <t>توضیحات</t>
+  </si>
+  <si>
+    <t>مثال: (این سطر پاک شود)</t>
+  </si>
+  <si>
+    <t>راهنما</t>
+  </si>
+  <si>
+    <t>فیلدهای ستاره دار الزامی است</t>
+  </si>
+  <si>
+    <t>عضویت در گروهها بصورت شناسه گروه نشان داده می شود</t>
+  </si>
+  <si>
+    <t>در صورت عضویت در چندین گروه، شناسه گروهها با کاما (,) جدا شود</t>
+  </si>
+  <si>
+    <t>مقادیر status در صورتی که مقادیر زیر وارد شود معتبر است:</t>
+  </si>
+  <si>
+    <t>employeeNumber</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>1234568sda</t>
+  </si>
+  <si>
+    <t>09123456789</t>
+  </si>
+  <si>
+    <t>#Parrsoo2020#</t>
+  </si>
+  <si>
+    <t>disable</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>Managers, Staff</t>
+  </si>
+  <si>
     <t>ali</t>
-  </si>
-  <si>
-    <t>amiri</t>
-  </si>
-  <si>
-    <t>علی امیری</t>
-  </si>
-  <si>
-    <t>ali.amiri@yahoo.com</t>
-  </si>
-  <si>
-    <t>توضیحات</t>
-  </si>
-  <si>
-    <t>مثال: (این سطر پاک شود)</t>
-  </si>
-  <si>
-    <t>راهنما</t>
-  </si>
-  <si>
-    <t>فیلدهای ستاره دار الزامی است</t>
-  </si>
-  <si>
-    <t>عضویت در گروهها بصورت شناسه گروه نشان داده می شود</t>
-  </si>
-  <si>
-    <t>در صورت عضویت در چندین گروه، شناسه گروهها با کاما (,) جدا شود</t>
-  </si>
-  <si>
-    <t>مقادیر status در صورتی که مقادیر زیر وارد شود معتبر است:</t>
-  </si>
-  <si>
-    <t>employeeNumber</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>1234568sda</t>
-  </si>
-  <si>
-    <t>09123456789</t>
-  </si>
-  <si>
-    <t>EndTime</t>
-  </si>
-  <si>
-    <t>#Parrsoo2020#</t>
-  </si>
-  <si>
-    <t>disable</t>
-  </si>
-  <si>
-    <t>enable</t>
-  </si>
-  <si>
-    <t>1400-10-20 13:13:13.259</t>
-  </si>
-  <si>
-    <t>Managers, Staff</t>
   </si>
 </sst>
 </file>
@@ -439,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -453,11 +447,10 @@
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="12.36328125" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" customWidth="1"/>
-    <col min="13" max="13" width="45.6328125" customWidth="1"/>
+    <col min="12" max="12" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,117 +479,111 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="M5" s="8" t="s">
-        <v>16</v>
+      <c r="L5" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="M6" s="9" t="s">
-        <v>17</v>
+      <c r="L6" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="M7" s="9" t="s">
-        <v>18</v>
+      <c r="L7" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B8" s="7"/>
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="M8" s="9" t="s">
-        <v>19</v>
+      <c r="L8" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="M9" s="9" t="s">
-        <v>20</v>
+      <c r="L9" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M10" s="10" t="s">
-        <v>28</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L10" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M11" s="10" t="s">
-        <v>27</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L11" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M12" s="10"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M13" s="11"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L13" s="11"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
All Export .xls File Names Changed to .xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Code\IDMAN\Code\src\main\resources\static\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maziy\Work\parsso-idma\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1FDB0A-C179-4492-B476-D3B52344C18F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83123F10-EEBB-4431-8846-7C19B268D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>userId*</t>
   </si>
@@ -97,9 +97,6 @@
     <t>09123456789</t>
   </si>
   <si>
-    <t>EndTime</t>
-  </si>
-  <si>
     <t>#Parrsoo2020#</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>enable</t>
-  </si>
-  <si>
-    <t>1400-10-20 13:13:13.259</t>
   </si>
   <si>
     <t>Managers, Staff</t>
@@ -439,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -453,11 +447,10 @@
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="12.36328125" customWidth="1"/>
-    <col min="12" max="12" width="21.54296875" customWidth="1"/>
-    <col min="13" max="13" width="45.6328125" customWidth="1"/>
+    <col min="12" max="12" width="45.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,14 +484,11 @@
       <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -518,85 +508,82 @@
         <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="M5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="M6" s="9" t="s">
+      <c r="L6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="M7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B8" s="7"/>
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="M8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="M9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M10" s="10" t="s">
-        <v>28</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L10" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M11" s="10" t="s">
-        <v>27</v>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L11" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M12" s="10"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="M13" s="11"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L13" s="11"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
minor fix on service update
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da1933711cb19495/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maziy\Work\parsso-idma\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{C2067E39-2B06-4FD4-A39F-3B3C2D2880FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A20464F-D34E-4517-ADCE-4C3E5165109D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83123F10-EEBB-4431-8846-7C19B268D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,6 +52,9 @@
     <t>این سطر را پاک نکنید(Don't remove)</t>
   </si>
   <si>
+    <t>ali</t>
+  </si>
+  <si>
     <t>amiri</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>Managers, Staff</t>
-  </si>
-  <si>
-    <t>ali</t>
   </si>
 </sst>
 </file>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -479,10 +479,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -490,40 +490,40 @@
     </row>
     <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
@@ -537,21 +537,21 @@
       <c r="D5" s="7"/>
       <c r="H5" s="7"/>
       <c r="L5" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D6" s="7"/>
       <c r="H6" s="7"/>
       <c r="L6" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D7" s="7"/>
       <c r="H7" s="7"/>
       <c r="L7" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
@@ -559,24 +559,24 @@
       <c r="D8" s="7"/>
       <c r="H8" s="7"/>
       <c r="L8" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="D9" s="7"/>
       <c r="H9" s="7"/>
       <c r="L9" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="L10" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="L11" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Public message problem fixed
</commit_message>
<xml_diff>
--- a/src/main/resources/static/template/users.xlsx
+++ b/src/main/resources/static/template/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maziy\Work\parsso-idma\src\main\resources\static\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maziy\IdeaProjects\IDMAN\src\main\resources\static\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83123F10-EEBB-4431-8846-7C19B268D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC17E75B-AE69-45DC-B055-391ABA0271A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -435,19 +435,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="5" max="5" width="11.2265625" style="14"/>
+    <col min="1" max="4" width="11.2265625" customWidth="1"/>
+    <col min="5" max="5" width="11.2265625" style="14" customWidth="1"/>
     <col min="6" max="6" width="18.6796875" customWidth="1"/>
     <col min="7" max="7" width="15.40625" customWidth="1"/>
+    <col min="8" max="8" width="11.2265625" customWidth="1"/>
     <col min="9" max="9" width="6.7265625" customWidth="1"/>
     <col min="10" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="12.36328125" customWidth="1"/>
     <col min="12" max="12" width="45.6328125" customWidth="1"/>
+    <col min="13" max="16384" width="11.2265625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">

</xml_diff>